<commit_message>
Tåler ikkje at det er meir grupper enn folk som har svart på ein oppgåve
</commit_message>
<xml_diff>
--- a/TicksSheet/Student-Led Tutorial #1.download.xlsx
+++ b/TicksSheet/Student-Led Tutorial #1.download.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Teaching\ELET1002\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sambaad.stud.ntnu.no\adriaeik\Documents\GitHub\ELET1002_Groups\TicksSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86F2B344-3A66-456F-8CFE-9041F34E68EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2D1DEF-8B82-432F-B829-B944CD5A97B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{48709412-FB9E-45C7-B4A1-E4433916C9C1}"/>
+    <workbookView xWindow="33255" yWindow="3810" windowWidth="21600" windowHeight="11385" xr2:uid="{48709412-FB9E-45C7-B4A1-E4433916C9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Student-Led Tutorial #1.downloa" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
   <si>
     <t>Username</t>
   </si>
@@ -1174,13 +1174,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FF108B-2013-4444-AC15-08CC8E96EEA7}">
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AO14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AP10" sqref="AP10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1303,11 @@
       <c r="AN1" t="s">
         <v>39</v>
       </c>
+      <c r="AO1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1405,8 +1410,11 @@
       <c r="AM2">
         <v>0</v>
       </c>
+      <c r="AO2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1509,8 +1517,11 @@
       <c r="AM3">
         <v>0</v>
       </c>
+      <c r="AO3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1613,8 +1624,11 @@
       <c r="AM4">
         <v>0</v>
       </c>
+      <c r="AO4" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1717,8 +1731,11 @@
       <c r="AM5">
         <v>1</v>
       </c>
+      <c r="AO5" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1821,8 +1838,11 @@
       <c r="AM6">
         <v>1</v>
       </c>
+      <c r="AO6" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1925,8 +1945,11 @@
       <c r="AM7">
         <v>0</v>
       </c>
+      <c r="AO7" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -2029,8 +2052,11 @@
       <c r="AM8">
         <v>0</v>
       </c>
+      <c r="AO8" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -2133,8 +2159,11 @@
       <c r="AM9">
         <v>1</v>
       </c>
+      <c r="AO9" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -2237,8 +2266,11 @@
       <c r="AM10">
         <v>0</v>
       </c>
+      <c r="AO10" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2341,8 +2373,11 @@
       <c r="AM11">
         <v>1</v>
       </c>
+      <c r="AO11" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -2445,8 +2480,11 @@
       <c r="AM12">
         <v>1</v>
       </c>
+      <c r="AO12" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -2549,8 +2587,11 @@
       <c r="AM13">
         <v>1</v>
       </c>
+      <c r="AO13" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -2651,6 +2692,9 @@
         <v>1</v>
       </c>
       <c r="AM14">
+        <v>1</v>
+      </c>
+      <c r="AO14" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>